<commit_message>
New Search tests for Q2 added
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Check_That_UserCanSearchForANewAdded_GF_Synonyms.xlsx
+++ b/src/main/resources/testdata/Check_That_UserCanSearchForANewAdded_GF_Synonyms.xlsx
@@ -11,13 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Data#</t>
   </si>
@@ -47,6 +46,12 @@
   </si>
   <si>
     <t>symbol</t>
+  </si>
+  <si>
+    <t>Acetobacter xylinum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sourcespecies </t>
   </si>
 </sst>
 </file>
@@ -388,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,7 +421,7 @@
     <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -432,8 +437,14 @@
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -448,6 +459,12 @@
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing the changes made in the files.
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata/Check_That_UserCanSearchForANewAdded_GF_Synonyms.xlsx
+++ b/src/main/resources/testdata/Check_That_UserCanSearchForANewAdded_GF_Synonyms.xlsx
@@ -57,7 +57,7 @@
     <t>GF_synonyms</t>
   </si>
   <si>
-    <t>gfsynonyms</t>
+    <t>gf_synonyms</t>
   </si>
 </sst>
 </file>
@@ -401,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>